<commit_message>
Change E_H2CC to E_H2NGCT
Prior to this commit, we defined a hydrogen combined cycle turbine (E_H2CC)
with the same specs as the natural gas combined cycle turbine, only it used
H2 as a fuel. This was based off a representation in the Open Energy Outlook.

We have updated that using data from the 2022 Nova Scotia Power Evergreen IRP.
This new technology, E_H2NGCT, is a combustion turbine that can use either
natural gas or H2.
</commit_message>
<xml_diff>
--- a/Excel Workbooks/Industry.xlsx
+++ b/Excel Workbooks/Industry.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\Documents\ACES-Modelling-Tools\ACES-Git\ACES-Data\Excel Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CDFE36-968F-4E29-B01E-16DC4754A89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAD4029-3DBF-4B0F-8C96-A27367DD7F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" tabRatio="626" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies and Commodities" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Data Sources" sheetId="14" r:id="rId14"/>
     <sheet name="Conversion Factors" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="330">
   <si>
     <t>Technologies</t>
   </si>
@@ -1246,11 +1246,17 @@
   <si>
     <t>Calculated</t>
   </si>
+  <si>
+    <t>[25]</t>
+  </si>
+  <si>
+    <t>Bistline, John ET, and Geoffrey J. Blanford. "Impact of carbon dioxide removal technologies on deep decarbonization of the electric power sector." Nature Communications 12.1 (2021): 1-12.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -1350,7 +1356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1397,6 +1403,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1405,7 +1422,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1474,6 +1491,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1492,13 +1512,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Accent1 2 70" xfId="3"/>
+    <cellStyle name="20% - Accent1 2 70" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1962,7 +1983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D84"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
@@ -1977,11 +1998,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2001,7 +2022,7 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2012,7 +2033,7 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="42"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
@@ -2021,7 +2042,7 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="42"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -2030,7 +2051,7 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="41"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
@@ -2039,7 +2060,7 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="42"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -2048,7 +2069,7 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -2057,7 +2078,7 @@
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="41"/>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
@@ -2066,7 +2087,7 @@
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -2075,7 +2096,7 @@
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="41"/>
+      <c r="D11" s="42"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
@@ -2332,11 +2353,11 @@
       <c r="D39" s="2"/>
     </row>
     <row r="42" spans="2:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
     </row>
     <row r="43" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -2736,7 +2757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2796,7 +2817,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2840,7 +2861,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="2" t="s">
         <v>169</v>
       </c>
@@ -2882,7 +2903,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="2" t="s">
         <v>169</v>
       </c>
@@ -2924,7 +2945,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="2" t="s">
         <v>169</v>
       </c>
@@ -2966,7 +2987,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3010,7 +3031,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="2" t="s">
         <v>175</v>
       </c>
@@ -3052,7 +3073,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="2" t="s">
         <v>175</v>
       </c>
@@ -3094,7 +3115,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
@@ -3136,7 +3157,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="2" t="s">
         <v>175</v>
       </c>
@@ -3178,7 +3199,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3222,7 +3243,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="2" t="s">
         <v>176</v>
       </c>
@@ -3264,7 +3285,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="2" t="s">
         <v>176</v>
       </c>
@@ -3306,7 +3327,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="2" t="s">
         <v>176</v>
       </c>
@@ -3348,7 +3369,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3392,7 +3413,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="2" t="s">
         <v>177</v>
       </c>
@@ -3434,7 +3455,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="2" t="s">
         <v>177</v>
       </c>
@@ -3476,7 +3497,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3520,7 +3541,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="2" t="s">
         <v>178</v>
       </c>
@@ -3562,7 +3583,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="2" t="s">
         <v>178</v>
       </c>
@@ -3604,7 +3625,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="2" t="s">
         <v>178</v>
       </c>
@@ -3646,7 +3667,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="2" t="s">
         <v>178</v>
       </c>
@@ -3688,7 +3709,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="2" t="s">
         <v>178</v>
       </c>
@@ -3730,7 +3751,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3774,7 +3795,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="2" t="s">
         <v>179</v>
       </c>
@@ -3816,7 +3837,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="2" t="s">
         <v>179</v>
       </c>
@@ -3858,7 +3879,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="2" t="s">
         <v>179</v>
       </c>
@@ -3900,7 +3921,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="2" t="s">
         <v>179</v>
       </c>
@@ -3942,7 +3963,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="43" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -3984,7 +4005,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="2" t="s">
         <v>183</v>
       </c>
@@ -4024,7 +4045,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="43" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -4066,7 +4087,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="2" t="s">
         <v>183</v>
       </c>
@@ -4106,7 +4127,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="43" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -4148,7 +4169,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="2" t="s">
         <v>183</v>
       </c>
@@ -4252,7 +4273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4319,7 +4340,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -4376,7 +4397,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="28" t="s">
         <v>178</v>
       </c>
@@ -4431,7 +4452,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="28" t="s">
         <v>196</v>
       </c>
@@ -4486,7 +4507,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="28" t="s">
         <v>198</v>
       </c>
@@ -4541,7 +4562,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -4598,7 +4619,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="28" t="s">
         <v>178</v>
       </c>
@@ -4653,7 +4674,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="28" t="s">
         <v>196</v>
       </c>
@@ -4708,7 +4729,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="28" t="s">
         <v>198</v>
       </c>
@@ -4763,7 +4784,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="28" t="s">
@@ -4820,7 +4841,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="28" t="s">
         <v>178</v>
       </c>
@@ -4875,7 +4896,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="28" t="s">
         <v>196</v>
       </c>
@@ -4930,7 +4951,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="28" t="s">
         <v>198</v>
       </c>
@@ -5051,7 +5072,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -5234,7 +5255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5247,50 +5268,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
     </row>
     <row r="8" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5317,11 +5338,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5331,10 +5352,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -5526,6 +5547,14 @@
       </c>
       <c r="B25" s="2" t="s">
         <v>302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="58" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5537,7 +5566,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" location="rm"/>
+    <hyperlink ref="B14" r:id="rId1" location="rm" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5546,7 +5575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5591,7 +5620,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>177</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -5623,7 +5652,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
+      <c r="A3" s="46"/>
       <c r="B3" s="33" t="s">
         <v>313</v>
       </c>
@@ -5653,7 +5682,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="33" t="s">
         <v>314</v>
       </c>
@@ -5683,7 +5712,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="33" t="s">
         <v>315</v>
       </c>
@@ -5719,7 +5748,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="46" t="s">
         <v>178</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -5751,7 +5780,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="33" t="s">
         <v>313</v>
       </c>
@@ -5781,7 +5810,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="33" t="s">
         <v>314</v>
       </c>
@@ -5811,7 +5840,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="33" t="s">
         <v>315</v>
       </c>
@@ -5847,7 +5876,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>196</v>
       </c>
       <c r="B10" s="33" t="s">
@@ -5879,7 +5908,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="33" t="s">
         <v>313</v>
       </c>
@@ -5909,7 +5938,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="33" t="s">
         <v>314</v>
       </c>
@@ -5939,7 +5968,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="33" t="s">
         <v>315</v>
       </c>
@@ -5975,7 +6004,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="46" t="s">
         <v>197</v>
       </c>
       <c r="B14" s="33" t="s">
@@ -6007,7 +6036,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="33" t="s">
         <v>313</v>
       </c>
@@ -6037,7 +6066,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="33" t="s">
         <v>314</v>
       </c>
@@ -6067,7 +6096,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="45"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="33" t="s">
         <v>315</v>
       </c>
@@ -6103,7 +6132,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="2" t="s">
         <v>316</v>
       </c>
@@ -6133,7 +6162,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="45"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="2" t="s">
         <v>317</v>
       </c>
@@ -6170,7 +6199,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="2" t="s">
         <v>318</v>
       </c>
@@ -6207,7 +6236,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="46" t="s">
         <v>319</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -6239,7 +6268,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="2" t="s">
         <v>321</v>
       </c>
@@ -6276,7 +6305,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="2" t="s">
         <v>322</v>
       </c>
@@ -6314,12 +6343,12 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="45" t="s">
         <v>324</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -6411,12 +6440,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="6">
+    <mergeCell ref="A28:D28"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6425,11 +6454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6822,7 +6851,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -6866,7 +6895,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="4" t="s">
         <v>180</v>
       </c>
@@ -6913,7 +6942,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -6955,7 +6984,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="4" t="s">
         <v>180</v>
       </c>
@@ -7002,7 +7031,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -7044,7 +7073,7 @@
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="4" t="s">
         <v>183</v>
       </c>
@@ -7089,7 +7118,7 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="4" t="s">
         <v>183</v>
       </c>
@@ -7136,7 +7165,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="43" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -7178,7 +7207,7 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="4" t="s">
         <v>183</v>
       </c>
@@ -7223,7 +7252,7 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="4" t="s">
         <v>183</v>
       </c>
@@ -7270,7 +7299,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="43" t="s">
         <v>59</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -7312,7 +7341,7 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="4" t="s">
         <v>183</v>
       </c>
@@ -7357,7 +7386,7 @@
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="4" t="s">
         <v>183</v>
       </c>
@@ -7446,7 +7475,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="43" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -7488,7 +7517,7 @@
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="4" t="s">
         <v>183</v>
       </c>
@@ -7535,7 +7564,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="43" t="s">
         <v>70</v>
       </c>
       <c r="B26" t="s">
@@ -7575,7 +7604,7 @@
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="4" t="s">
         <v>183</v>
       </c>
@@ -7621,8 +7650,89 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="L28" s="5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+    </row>
+    <row r="29" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="43"/>
+      <c r="B29" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>328</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H29" s="5">
+        <f>H28*'Conversion Factors'!E$23</f>
+        <v>0.77978000000000003</v>
+      </c>
+      <c r="I29" s="5">
+        <f>I28*'Conversion Factors'!F$23</f>
+        <v>0.76136000000000004</v>
+      </c>
+      <c r="J29" s="5">
+        <f>J28*'Conversion Factors'!G$23</f>
+        <v>0.75522</v>
+      </c>
+      <c r="K29" s="5">
+        <f>K28*'Conversion Factors'!H$23</f>
+        <v>0.74907999999999997</v>
+      </c>
+      <c r="L29" s="5">
+        <f>L28*'Conversion Factors'!I$23</f>
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+    </row>
     <row r="30" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7668,10 +7778,10 @@
     <row r="72" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
@@ -7687,7 +7797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -7746,7 +7856,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -7798,7 +7908,7 @@
       <c r="Y2" s="10"/>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="2" t="s">
         <v>177</v>
       </c>
@@ -7846,7 +7956,7 @@
       <c r="Y3" s="10"/>
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="2" t="s">
         <v>196</v>
       </c>
@@ -7889,7 +7999,7 @@
       <c r="Y4" s="10"/>
     </row>
     <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="2" t="s">
         <v>197</v>
       </c>
@@ -7933,7 +8043,7 @@
       <c r="W5" s="11"/>
     </row>
     <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="2" t="s">
         <v>198</v>
       </c>
@@ -7984,7 +8094,7 @@
       <c r="Y6" s="10"/>
     </row>
     <row r="7" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="2" t="s">
         <v>200</v>
       </c>
@@ -8023,7 +8133,7 @@
       <c r="Y7" s="10"/>
     </row>
     <row r="8" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="43" t="s">
         <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -8073,7 +8183,7 @@
       <c r="Y8" s="10"/>
     </row>
     <row r="9" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="2" t="s">
         <v>177</v>
       </c>
@@ -8120,7 +8230,7 @@
       <c r="W9" s="11"/>
     </row>
     <row r="10" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="2" t="s">
         <v>196</v>
       </c>
@@ -8162,7 +8272,7 @@
       <c r="W10" s="11"/>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="2" t="s">
         <v>197</v>
       </c>
@@ -8211,7 +8321,7 @@
       <c r="Y11" s="10"/>
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="2" t="s">
         <v>198</v>
       </c>
@@ -8259,7 +8369,7 @@
       <c r="Y12" s="10"/>
     </row>
     <row r="13" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="2" t="s">
         <v>200</v>
       </c>
@@ -8307,7 +8417,7 @@
       <c r="W13" s="11"/>
     </row>
     <row r="14" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>103</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -8345,7 +8455,7 @@
       <c r="W14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="2" t="s">
         <v>177</v>
       </c>
@@ -8383,7 +8493,7 @@
       <c r="W15" s="8"/>
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="2" t="s">
         <v>196</v>
       </c>
@@ -8419,7 +8529,7 @@
       <c r="W16" s="11"/>
     </row>
     <row r="17" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="2" t="s">
         <v>197</v>
       </c>
@@ -8464,7 +8574,7 @@
       <c r="W17" s="11"/>
     </row>
     <row r="18" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="2" t="s">
         <v>198</v>
       </c>
@@ -8516,7 +8626,7 @@
       <c r="W18" s="8"/>
     </row>
     <row r="19" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="2" t="s">
         <v>200</v>
       </c>
@@ -8552,7 +8662,7 @@
       <c r="W19" s="11"/>
     </row>
     <row r="20" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="43" t="s">
         <v>109</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -8601,7 +8711,7 @@
       <c r="W20" s="11"/>
     </row>
     <row r="21" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="2" t="s">
         <v>177</v>
       </c>
@@ -8643,7 +8753,7 @@
       <c r="W21" s="11"/>
     </row>
     <row r="22" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="2" t="s">
         <v>196</v>
       </c>
@@ -8685,7 +8795,7 @@
       <c r="W22" s="11"/>
     </row>
     <row r="23" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="2" t="s">
         <v>197</v>
       </c>
@@ -8729,7 +8839,7 @@
       <c r="W23" s="11"/>
     </row>
     <row r="24" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="2" t="s">
         <v>198</v>
       </c>
@@ -8779,7 +8889,7 @@
       <c r="W24" s="8"/>
     </row>
     <row r="25" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="2" t="s">
         <v>200</v>
       </c>
@@ -8827,7 +8937,7 @@
       <c r="W25" s="11"/>
     </row>
     <row r="26" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="43" t="s">
         <v>93</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -8871,7 +8981,7 @@
       <c r="W26" s="11"/>
     </row>
     <row r="27" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="2" t="s">
         <v>177</v>
       </c>
@@ -8918,7 +9028,7 @@
       <c r="W27" s="11"/>
     </row>
     <row r="28" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="2" t="s">
         <v>196</v>
       </c>
@@ -8960,7 +9070,7 @@
       <c r="W28" s="11"/>
     </row>
     <row r="29" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="2" t="s">
         <v>197</v>
       </c>
@@ -9001,7 +9111,7 @@
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="2" t="s">
         <v>198</v>
       </c>
@@ -9037,7 +9147,7 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="2" t="s">
         <v>200</v>
       </c>
@@ -9072,7 +9182,7 @@
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="43" t="s">
         <v>107</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -9119,7 +9229,7 @@
       </c>
     </row>
     <row r="33" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="2" t="s">
         <v>177</v>
       </c>
@@ -9161,7 +9271,7 @@
       <c r="R33" s="10"/>
     </row>
     <row r="34" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="2" t="s">
         <v>196</v>
       </c>
@@ -9202,7 +9312,7 @@
       <c r="M34" s="2"/>
     </row>
     <row r="35" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="2" t="s">
         <v>197</v>
       </c>
@@ -9245,7 +9355,7 @@
       <c r="M35" s="2"/>
     </row>
     <row r="36" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="2" t="s">
         <v>198</v>
       </c>
@@ -9282,7 +9392,7 @@
       <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="2" t="s">
         <v>200</v>
       </c>
@@ -9319,7 +9429,7 @@
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="43" t="s">
         <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -9367,7 +9477,7 @@
       <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="42"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="2" t="s">
         <v>177</v>
       </c>
@@ -9413,7 +9523,7 @@
       <c r="O39" s="8"/>
     </row>
     <row r="40" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="42"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="2" t="s">
         <v>196</v>
       </c>
@@ -9459,7 +9569,7 @@
       <c r="O40" s="8"/>
     </row>
     <row r="41" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="2" t="s">
         <v>197</v>
       </c>
@@ -9502,7 +9612,7 @@
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="42"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="2" t="s">
         <v>198</v>
       </c>
@@ -9549,7 +9659,7 @@
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="2" t="s">
         <v>200</v>
       </c>
@@ -9596,7 +9706,7 @@
       <c r="O43" s="8"/>
     </row>
     <row r="44" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="43" t="s">
         <v>95</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -9643,7 +9753,7 @@
       </c>
     </row>
     <row r="45" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="42"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="2" t="s">
         <v>177</v>
       </c>
@@ -9688,7 +9798,7 @@
       </c>
     </row>
     <row r="46" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="42"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="2" t="s">
         <v>196</v>
       </c>
@@ -9733,7 +9843,7 @@
       </c>
     </row>
     <row r="47" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="42"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="2" t="s">
         <v>197</v>
       </c>
@@ -9776,7 +9886,7 @@
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="42"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="2" t="s">
         <v>198</v>
       </c>
@@ -9822,7 +9932,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="2" t="s">
         <v>200</v>
       </c>
@@ -9868,7 +9978,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="43" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -9915,7 +10025,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="2" t="s">
         <v>177</v>
       </c>
@@ -9960,7 +10070,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="42"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="2" t="s">
         <v>196</v>
       </c>
@@ -10005,7 +10115,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="2" t="s">
         <v>197</v>
       </c>
@@ -10048,7 +10158,7 @@
       <c r="M53" s="2"/>
     </row>
     <row r="54" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="42"/>
+      <c r="A54" s="43"/>
       <c r="B54" s="2" t="s">
         <v>198</v>
       </c>
@@ -10094,7 +10204,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="42"/>
+      <c r="A55" s="43"/>
       <c r="B55" s="2" t="s">
         <v>200</v>
       </c>
@@ -10159,7 +10269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -10218,7 +10328,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -10258,7 +10368,7 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="4" t="s">
         <v>180</v>
       </c>
@@ -10305,7 +10415,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -10345,7 +10455,7 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="4" t="s">
         <v>180</v>
       </c>
@@ -10392,7 +10502,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -10434,7 +10544,7 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="2" t="s">
         <v>183</v>
       </c>
@@ -10479,7 +10589,7 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="2" t="s">
         <v>183</v>
       </c>
@@ -10526,7 +10636,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="43" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -10568,7 +10678,7 @@
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="2" t="s">
         <v>183</v>
       </c>
@@ -10613,7 +10723,7 @@
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="2" t="s">
         <v>183</v>
       </c>
@@ -10660,7 +10770,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="43" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -10702,7 +10812,7 @@
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="2" t="s">
         <v>183</v>
       </c>
@@ -10747,7 +10857,7 @@
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="2" t="s">
         <v>183</v>
       </c>
@@ -10794,7 +10904,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="43" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -10836,7 +10946,7 @@
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="2" t="s">
         <v>183</v>
       </c>
@@ -10883,7 +10993,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="43" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -10923,7 +11033,7 @@
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="2" t="s">
         <v>183</v>
       </c>
@@ -11086,7 +11196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N89"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -11144,7 +11254,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>212</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -11186,7 +11296,7 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="2" t="s">
         <v>179</v>
       </c>
@@ -11233,7 +11343,7 @@
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="2" t="s">
         <v>179</v>
       </c>
@@ -11282,7 +11392,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -11324,7 +11434,7 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="2" t="s">
         <v>179</v>
       </c>
@@ -11371,7 +11481,7 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="2" t="s">
         <v>179</v>
       </c>
@@ -11420,7 +11530,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="43" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -11462,7 +11572,7 @@
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="2" t="s">
         <v>179</v>
       </c>
@@ -11509,7 +11619,7 @@
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="2" t="s">
         <v>179</v>
       </c>
@@ -11558,7 +11668,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -11600,7 +11710,7 @@
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="2" t="s">
         <v>179</v>
       </c>
@@ -11647,7 +11757,7 @@
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="2" t="s">
         <v>179</v>
       </c>
@@ -11696,7 +11806,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -11738,7 +11848,7 @@
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="2" t="s">
         <v>179</v>
       </c>
@@ -11785,7 +11895,7 @@
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="2" t="s">
         <v>179</v>
       </c>
@@ -11834,7 +11944,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="43" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -11876,7 +11986,7 @@
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="2" t="s">
         <v>217</v>
       </c>
@@ -11923,7 +12033,7 @@
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="2" t="s">
         <v>217</v>
       </c>
@@ -11972,7 +12082,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -12014,7 +12124,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="2" t="s">
         <v>177</v>
       </c>
@@ -12061,7 +12171,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="2" t="s">
         <v>177</v>
       </c>
@@ -12238,7 +12348,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -12278,7 +12388,7 @@
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="4" t="s">
         <v>180</v>
       </c>
@@ -12325,7 +12435,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -12365,7 +12475,7 @@
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="4" t="s">
         <v>180</v>
       </c>
@@ -12412,7 +12522,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -12452,7 +12562,7 @@
       <c r="N30" s="2"/>
     </row>
     <row r="31" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="2" t="s">
         <v>179</v>
       </c>
@@ -12499,7 +12609,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="43" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -12539,7 +12649,7 @@
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="2" t="s">
         <v>179</v>
       </c>
@@ -12586,7 +12696,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -12626,7 +12736,7 @@
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="2" t="s">
         <v>179</v>
       </c>
@@ -12673,7 +12783,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="43" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -12715,7 +12825,7 @@
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="2" t="s">
         <v>183</v>
       </c>
@@ -12995,6 +13105,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A26:A27"/>
@@ -13002,12 +13118,6 @@
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -13016,7 +13126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13682,7 +13792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
@@ -13746,7 +13856,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -13789,7 +13899,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="2" t="s">
         <v>169</v>
       </c>
@@ -13830,7 +13940,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="2" t="s">
         <v>169</v>
       </c>
@@ -13871,7 +13981,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="2" t="s">
         <v>169</v>
       </c>
@@ -13912,7 +14022,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -13955,7 +14065,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="2" t="s">
         <v>175</v>
       </c>
@@ -13996,7 +14106,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="2" t="s">
         <v>175</v>
       </c>
@@ -14037,7 +14147,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
@@ -14078,7 +14188,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="2" t="s">
         <v>175</v>
       </c>
@@ -14168,7 +14278,7 @@
       <c r="S11" s="23"/>
     </row>
     <row r="12" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -14213,7 +14323,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="2" t="s">
         <v>176</v>
       </c>
@@ -14254,7 +14364,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="2" t="s">
         <v>176</v>
       </c>
@@ -14295,7 +14405,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="2" t="s">
         <v>176</v>
       </c>
@@ -14336,7 +14446,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -14379,7 +14489,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="2" t="s">
         <v>177</v>
       </c>
@@ -14420,7 +14530,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="2" t="s">
         <v>177</v>
       </c>
@@ -14461,7 +14571,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -14504,7 +14614,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="2" t="s">
         <v>178</v>
       </c>
@@ -14545,7 +14655,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="2" t="s">
         <v>178</v>
       </c>
@@ -14586,7 +14696,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="2" t="s">
         <v>178</v>
       </c>
@@ -14627,7 +14737,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="2" t="s">
         <v>178</v>
       </c>
@@ -14668,7 +14778,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="2" t="s">
         <v>178</v>
       </c>
@@ -14709,7 +14819,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -14752,7 +14862,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="2" t="s">
         <v>179</v>
       </c>
@@ -14793,7 +14903,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="2" t="s">
         <v>179</v>
       </c>
@@ -14834,7 +14944,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="2" t="s">
         <v>179</v>
       </c>
@@ -14875,7 +14985,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="2" t="s">
         <v>179</v>
       </c>
@@ -15684,7 +15794,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="42" t="s">
+      <c r="A48" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -15727,7 +15837,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="4" t="s">
         <v>180</v>
       </c>
@@ -15768,7 +15878,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -15811,7 +15921,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="4" t="s">
         <v>180</v>
       </c>
@@ -15852,7 +15962,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="43" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -15895,7 +16005,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="2" t="s">
         <v>183</v>
       </c>
@@ -16110,7 +16220,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="42" t="s">
+      <c r="A58" s="43" t="s">
         <v>64</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -16155,7 +16265,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="42"/>
+      <c r="A59" s="43"/>
       <c r="B59" s="2" t="s">
         <v>183</v>
       </c>
@@ -16333,7 +16443,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="42" t="s">
+      <c r="A63" s="43" t="s">
         <v>70</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -16378,7 +16488,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="42"/>
+      <c r="A64" s="43"/>
       <c r="B64" s="2" t="s">
         <v>183</v>
       </c>
@@ -16466,7 +16576,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="42" t="s">
+      <c r="A66" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -16511,7 +16621,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="42"/>
+      <c r="A67" s="43"/>
       <c r="B67" s="2" t="s">
         <v>183</v>
       </c>
@@ -16626,11 +16736,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A10"/>
@@ -16638,6 +16743,11 @@
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16646,7 +16756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -17532,11 +17642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17599,7 +17709,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -17647,7 +17757,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>247</v>
@@ -17698,7 +17808,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>247</v>
@@ -17749,7 +17859,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>247</v>
@@ -17802,7 +17912,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -17850,7 +17960,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>247</v>
@@ -17901,7 +18011,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>247</v>
@@ -17952,7 +18062,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>247</v>
@@ -18005,7 +18115,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -18053,7 +18163,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>247</v>
@@ -18104,7 +18214,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>247</v>
@@ -18155,7 +18265,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>247</v>
@@ -18208,7 +18318,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -18256,7 +18366,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>247</v>
@@ -18307,7 +18417,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>247</v>
@@ -18358,7 +18468,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>247</v>
@@ -18411,7 +18521,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="43" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -18459,7 +18569,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>247</v>
@@ -18510,7 +18620,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>247</v>
@@ -18561,7 +18671,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>247</v>
@@ -18614,7 +18724,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -18662,7 +18772,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>247</v>
@@ -18706,7 +18816,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>247</v>
@@ -18757,7 +18867,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>247</v>
@@ -18810,7 +18920,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="43" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -18858,7 +18968,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>247</v>
@@ -18902,7 +19012,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>247</v>
@@ -18953,7 +19063,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>247</v>
@@ -19006,7 +19116,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="43" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -19054,7 +19164,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>247</v>
@@ -19105,7 +19215,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>247</v>
@@ -19156,7 +19266,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>247</v>
@@ -19209,7 +19319,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -19259,7 +19369,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
         <v>250</v>
@@ -19312,7 +19422,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -19362,7 +19472,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>181</v>
@@ -19406,7 +19516,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
         <v>181</v>
@@ -19450,7 +19560,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="42"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
         <v>181</v>
@@ -19494,7 +19604,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -19542,7 +19652,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
         <v>181</v>
@@ -19586,7 +19696,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="42"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
         <v>181</v>
@@ -19630,7 +19740,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
         <v>181</v>
@@ -19674,7 +19784,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="43" t="s">
         <v>55</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -19722,7 +19832,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="42"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
         <v>184</v>
@@ -19766,100 +19876,44 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="40"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="40"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="43" t="s">
         <v>57</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="J46" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K46" s="2">
-        <v>-1</v>
-      </c>
-      <c r="L46" s="2">
-        <v>-1</v>
-      </c>
-      <c r="M46" s="2">
-        <v>-1</v>
-      </c>
-      <c r="N46" s="2">
-        <v>-1</v>
-      </c>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="42"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="I47" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="J47" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K47" s="2">
-        <v>-1</v>
-      </c>
-      <c r="L47" s="2">
-        <v>-1</v>
-      </c>
-      <c r="M47" s="2">
-        <v>-1</v>
-      </c>
-      <c r="N47" s="2">
-        <v>-1</v>
-      </c>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="42" t="s">
-        <v>59</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>183</v>
@@ -19906,7 +19960,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
         <v>184</v>
@@ -19949,14 +20003,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="42" t="s">
-        <v>61</v>
+    <row r="50" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="43" t="s">
+        <v>59</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>183</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="D50" s="2" t="s">
         <v>253</v>
       </c>
@@ -19964,16 +20020,16 @@
         <v>155</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H50" s="2">
-        <v>-1</v>
-      </c>
-      <c r="I50" s="2">
-        <v>-1</v>
+        <v>83</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>173</v>
       </c>
       <c r="J50" s="2">
         <v>-1</v>
@@ -19995,10 +20051,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
+    <row r="51" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="43"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="D51" s="2" t="s">
         <v>253</v>
       </c>
@@ -20006,16 +20064,16 @@
         <v>157</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H51" s="2">
-        <v>-1</v>
-      </c>
-      <c r="I51" s="2">
-        <v>-1</v>
+        <v>83</v>
+      </c>
+      <c r="H51" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I51" s="24" t="s">
+        <v>173</v>
       </c>
       <c r="J51" s="2">
         <v>-1</v>
@@ -20037,30 +20095,118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F54" s="10"/>
-    </row>
-    <row r="70" spans="5:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E70" s="10"/>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="43"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F56" s="10"/>
+    </row>
+    <row r="72" spans="5:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E72" s="10"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>